<commit_message>
Improved displayname of billing BIS v3
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$F$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$F$66</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="125">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.2::D16B</t>
+  </si>
+  <si>
+    <t>PEPPOL BIS Billing Invoice V3</t>
+  </si>
+  <si>
+    <t>PEPPOL BIS Billing CreditNote V3</t>
   </si>
 </sst>
 </file>
@@ -893,8 +899,8 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -1518,7 +1524,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="4" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>73</v>
@@ -1536,7 +1542,7 @@
     </row>
     <row r="33" spans="1:6" ht="29">
       <c r="A33" s="4" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>73</v>
@@ -2153,7 +2159,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F31"/>
+  <autoFilter ref="A1:F66"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Also added text on CII
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -186,9 +186,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0::2.1</t>
   </si>
   <si>
-    <t>PEPPOL BIS Billing V3</t>
-  </si>
-  <si>
     <t>DHSC Customized Ordering profile V1</t>
   </si>
   <si>
@@ -396,10 +393,13 @@
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.2::D16B</t>
   </si>
   <si>
-    <t>PEPPOL BIS Billing Invoice V3</t>
-  </si>
-  <si>
-    <t>PEPPOL BIS Billing CreditNote V3</t>
+    <t>PEPPOL BIS Billing UBL Invoice V3</t>
+  </si>
+  <si>
+    <t>PEPPOL BIS Billing UBL CreditNote V3</t>
+  </si>
+  <si>
+    <t>PEPPOL BIS Billing CII Invoice V3</t>
   </si>
 </sst>
 </file>
@@ -899,8 +899,8 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -917,13 +917,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
@@ -940,7 +940,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -961,7 +961,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -982,7 +982,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -1003,7 +1003,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
@@ -1024,7 +1024,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1045,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -1066,7 +1066,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
@@ -1084,7 +1084,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1105,10 +1105,10 @@
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>29</v>
@@ -1121,7 +1121,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="29">
@@ -1129,10 +1129,10 @@
         <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
@@ -1147,7 +1147,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -1168,7 +1168,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
@@ -1186,7 +1186,7 @@
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
@@ -1207,7 +1207,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -1228,7 +1228,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
@@ -1249,7 +1249,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>36</v>
@@ -1267,7 +1267,7 @@
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>37</v>
@@ -1285,7 +1285,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1303,7 +1303,7 @@
         <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1321,7 +1321,7 @@
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -1339,7 +1339,7 @@
         <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1357,7 +1357,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1375,7 +1375,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1393,7 +1393,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>23</v>
@@ -1414,7 +1414,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>25</v>
@@ -1432,7 +1432,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>43</v>
@@ -1450,7 +1450,7 @@
         <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>44</v>
@@ -1465,7 +1465,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="29">
@@ -1473,10 +1473,10 @@
         <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="8">
         <v>3</v>
@@ -1491,7 +1491,7 @@
         <v>45</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>47</v>
@@ -1509,7 +1509,7 @@
         <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>48</v>
@@ -1524,10 +1524,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>51</v>
@@ -1542,10 +1542,10 @@
     </row>
     <row r="33" spans="1:6" ht="29">
       <c r="A33" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>52</v>
@@ -1560,13 +1560,13 @@
     </row>
     <row r="34" spans="1:6" ht="43.5">
       <c r="A34" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="8">
         <v>3</v>
@@ -1578,13 +1578,13 @@
     </row>
     <row r="35" spans="1:6" ht="43.5">
       <c r="A35" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="8">
         <v>3</v>
@@ -1596,13 +1596,13 @@
     </row>
     <row r="36" spans="1:6" ht="29">
       <c r="A36" s="4" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" s="6">
         <v>3</v>
@@ -1614,13 +1614,13 @@
     </row>
     <row r="37" spans="1:6" ht="29">
       <c r="A37" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" s="6">
         <v>3</v>
@@ -1632,13 +1632,13 @@
     </row>
     <row r="38" spans="1:6" ht="29">
       <c r="A38" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D38" s="6">
         <v>3</v>
@@ -1650,13 +1650,13 @@
     </row>
     <row r="39" spans="1:6" ht="29">
       <c r="A39" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="6">
         <v>3</v>
@@ -1668,13 +1668,13 @@
     </row>
     <row r="40" spans="1:6" ht="29">
       <c r="A40" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D40" s="6">
         <v>3</v>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="41" spans="1:6" ht="29">
       <c r="A41" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" s="6">
         <v>3</v>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="42" spans="1:6" ht="29">
       <c r="A42" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42" s="6">
         <v>3</v>
@@ -1722,13 +1722,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="D43" s="10">
         <v>3</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="44" spans="1:6" ht="29">
       <c r="A44" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="D44" s="10">
         <v>3</v>
@@ -1762,13 +1762,13 @@
     </row>
     <row r="45" spans="1:6" ht="29">
       <c r="A45" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" s="10">
         <v>3</v>
@@ -1782,13 +1782,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="10">
         <v>3</v>
@@ -1800,13 +1800,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D47" s="10">
         <v>3</v>
@@ -1818,13 +1818,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D48" s="10">
         <v>3</v>
@@ -1836,13 +1836,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D49" s="10">
         <v>3</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D50" s="6">
         <v>4</v>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D51" s="10">
         <v>4</v>
@@ -1890,13 +1890,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D52" s="10">
         <v>4</v>
@@ -1908,13 +1908,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D53" s="10">
         <v>4</v>
@@ -1926,13 +1926,13 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D54" s="10">
         <v>4</v>
@@ -1944,13 +1944,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D55" s="10">
         <v>4</v>
@@ -1962,13 +1962,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D56" s="10">
         <v>4</v>
@@ -1980,13 +1980,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D57" s="10">
         <v>4</v>
@@ -1998,13 +1998,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D58" s="10">
         <v>4</v>
@@ -2016,13 +2016,13 @@
     </row>
     <row r="59" spans="1:5" ht="29">
       <c r="A59" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D59" s="10">
         <v>4</v>
@@ -2034,13 +2034,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="D60" s="10">
         <v>4</v>
@@ -2052,13 +2052,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="D61" s="10">
         <v>4</v>
@@ -2070,13 +2070,13 @@
     </row>
     <row r="62" spans="1:5" ht="29">
       <c r="A62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D62" s="10">
         <v>4</v>
@@ -2088,13 +2088,13 @@
     </row>
     <row r="63" spans="1:5" ht="29">
       <c r="A63" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="D63" s="10">
         <v>4</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D64" s="6">
         <v>5</v>
@@ -2124,13 +2124,13 @@
     </row>
     <row r="65" spans="1:5" ht="29">
       <c r="A65" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D65" s="6">
         <v>5</v>
@@ -2142,13 +2142,13 @@
     </row>
     <row r="66" spans="1:5" ht="29">
       <c r="A66" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D66" s="6">
         <v>5</v>

</xml_diff>

<commit_message>
Changed the Profile code of several document types so that they come closer to uniqueness
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="133">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -132,27 +132,18 @@
     <t>PEPPOL Billing profile V1</t>
   </si>
   <si>
-    <t>PEPPOL Billing profile V2</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:www.cenbii.eu:transaction:biitrns010:ver2.0:extended:urn:www.peppol.eu:bis:peppol5a:ver2.0::2.1</t>
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:www.cenbii.eu:transaction:biitrns014:ver2.0:extended:urn:www.peppol.eu:bis:peppol5a:ver2.0::2.1</t>
   </si>
   <si>
-    <t>PEPPOL Procurement profile V1</t>
-  </si>
-  <si>
     <t>EHF Invoice V1</t>
   </si>
   <si>
     <t>Standalone Credit Note according to EHF V1</t>
   </si>
   <si>
-    <t>PEPPOL Ordering profile V1</t>
-  </si>
-  <si>
     <t>PEPPOL Catalogue profile V4</t>
   </si>
   <si>
@@ -186,12 +177,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0::2.1</t>
   </si>
   <si>
-    <t>DHSC Customized Ordering profile V1</t>
-  </si>
-  <si>
-    <t>DHSC Customized  Ordering profile V1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biitrns001:ver2.0:extended:urn:www.peppol.eu:bis:peppol28a:ver1.0:extended:urn:fdc:peppol-authority.co.uk:spec:ordering:ver1.0::2.1</t>
   </si>
   <si>
@@ -207,15 +192,6 @@
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0::D16B</t>
   </si>
   <si>
-    <t>Procurement procedure subscription V1</t>
-  </si>
-  <si>
-    <t>Procurement document access V1</t>
-  </si>
-  <si>
-    <t>Tender Submission V1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ExpressionOfInterestRequest-2::ExpressionOfInterestRequest##urn:www.cenbii.eu:transaction:biitrdm081:ver3.0:extended:urn:fdc:peppol.eu:2017:pracc:t001:ver1.0::2.2</t>
   </si>
   <si>
@@ -400,6 +376,54 @@
   </si>
   <si>
     <t>PEPPOL BIS Billing CII Invoice V3</t>
+  </si>
+  <si>
+    <t>PEPPOL Billing profile Invoice V2</t>
+  </si>
+  <si>
+    <t>PEPPOL Billing profile CreditNote V2</t>
+  </si>
+  <si>
+    <t>Tender Submission TenderReceipt V1</t>
+  </si>
+  <si>
+    <t>Tender Submission Tender V1</t>
+  </si>
+  <si>
+    <t>Procurement document access CallForTenders V1</t>
+  </si>
+  <si>
+    <t>Procurement document access TenderStatusRequest V1</t>
+  </si>
+  <si>
+    <t>Procurement procedure subscription Response V1</t>
+  </si>
+  <si>
+    <t>Procurement procedure subscription Request V1</t>
+  </si>
+  <si>
+    <t>DHSC Customized  Ordering profile OrderResponse V1</t>
+  </si>
+  <si>
+    <t>DHSC Customized Ordering profile Order V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Ordering profile Order V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Ordering profile OrderResponse V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Procurement profile Order V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Procurement profile OrderResponseSimple V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Procurement profile Invoice V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Procurement profile CreditNote V1</t>
   </si>
 </sst>
 </file>
@@ -899,13 +923,13 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.6328125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="129.26953125" style="4" customWidth="1"/>
     <col min="4" max="4" width="8" style="6" bestFit="1" customWidth="1"/>
@@ -917,22 +941,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="29">
@@ -940,7 +964,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -961,7 +985,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -982,7 +1006,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -1003,7 +1027,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
@@ -1024,7 +1048,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1045,7 +1069,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -1063,10 +1087,10 @@
     </row>
     <row r="8" spans="1:7" ht="29">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
@@ -1084,7 +1108,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1105,10 +1129,10 @@
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>29</v>
@@ -1121,7 +1145,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="29">
@@ -1129,10 +1153,10 @@
         <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
@@ -1147,7 +1171,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
@@ -1168,7 +1192,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
@@ -1186,7 +1210,7 @@
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
@@ -1207,7 +1231,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -1228,7 +1252,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
@@ -1246,13 +1270,13 @@
     </row>
     <row r="17" spans="1:7" ht="29">
       <c r="A17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>29</v>
@@ -1264,13 +1288,13 @@
     </row>
     <row r="18" spans="1:7" ht="29">
       <c r="A18" s="2" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>29</v>
@@ -1282,10 +1306,10 @@
     </row>
     <row r="19" spans="1:7" ht="29">
       <c r="A19" s="4" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1300,10 +1324,10 @@
     </row>
     <row r="20" spans="1:7" ht="29">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1318,10 +1342,10 @@
     </row>
     <row r="21" spans="1:7" ht="29">
       <c r="A21" s="4" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -1336,10 +1360,10 @@
     </row>
     <row r="22" spans="1:7" ht="29">
       <c r="A22" s="4" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1354,10 +1378,10 @@
     </row>
     <row r="23" spans="1:7" ht="29">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1372,10 +1396,10 @@
     </row>
     <row r="24" spans="1:7" ht="29">
       <c r="A24" s="4" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1390,10 +1414,10 @@
     </row>
     <row r="25" spans="1:7" ht="29">
       <c r="A25" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>23</v>
@@ -1411,10 +1435,10 @@
     </row>
     <row r="26" spans="1:7" ht="43.5">
       <c r="A26" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>25</v>
@@ -1429,13 +1453,13 @@
     </row>
     <row r="27" spans="1:7" ht="29">
       <c r="A27" s="4" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>29</v>
@@ -1447,13 +1471,13 @@
     </row>
     <row r="28" spans="1:7" ht="29">
       <c r="A28" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>29</v>
@@ -1465,18 +1489,18 @@
         <v>3</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="29">
       <c r="A29" s="4" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D29" s="8">
         <v>3</v>
@@ -1488,13 +1512,13 @@
     </row>
     <row r="30" spans="1:7" ht="29">
       <c r="A30" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>29</v>
@@ -1506,13 +1530,13 @@
     </row>
     <row r="31" spans="1:7" ht="29">
       <c r="A31" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>29</v>
@@ -1524,13 +1548,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="4" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D32" s="6">
         <v>2</v>
@@ -1542,13 +1566,13 @@
     </row>
     <row r="33" spans="1:6" ht="29">
       <c r="A33" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D33" s="6">
         <v>2</v>
@@ -1560,13 +1584,13 @@
     </row>
     <row r="34" spans="1:6" ht="43.5">
       <c r="A34" s="4" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D34" s="8">
         <v>3</v>
@@ -1578,13 +1602,13 @@
     </row>
     <row r="35" spans="1:6" ht="43.5">
       <c r="A35" s="4" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D35" s="8">
         <v>3</v>
@@ -1596,13 +1620,13 @@
     </row>
     <row r="36" spans="1:6" ht="29">
       <c r="A36" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D36" s="6">
         <v>3</v>
@@ -1614,13 +1638,13 @@
     </row>
     <row r="37" spans="1:6" ht="29">
       <c r="A37" s="10" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D37" s="6">
         <v>3</v>
@@ -1632,13 +1656,13 @@
     </row>
     <row r="38" spans="1:6" ht="29">
       <c r="A38" s="10" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D38" s="6">
         <v>3</v>
@@ -1650,13 +1674,13 @@
     </row>
     <row r="39" spans="1:6" ht="29">
       <c r="A39" s="10" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D39" s="6">
         <v>3</v>
@@ -1668,13 +1692,13 @@
     </row>
     <row r="40" spans="1:6" ht="29">
       <c r="A40" s="10" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D40" s="6">
         <v>3</v>
@@ -1686,13 +1710,13 @@
     </row>
     <row r="41" spans="1:6" ht="29">
       <c r="A41" s="10" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D41" s="6">
         <v>3</v>
@@ -1704,13 +1728,13 @@
     </row>
     <row r="42" spans="1:6" ht="29">
       <c r="A42" s="10" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D42" s="6">
         <v>3</v>
@@ -1722,13 +1746,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D43" s="10">
         <v>3</v>
@@ -1742,13 +1766,13 @@
     </row>
     <row r="44" spans="1:6" ht="29">
       <c r="A44" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D44" s="10">
         <v>3</v>
@@ -1762,13 +1786,13 @@
     </row>
     <row r="45" spans="1:6" ht="29">
       <c r="A45" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D45" s="10">
         <v>3</v>
@@ -1782,13 +1806,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D46" s="10">
         <v>3</v>
@@ -1800,13 +1824,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D47" s="10">
         <v>3</v>
@@ -1818,13 +1842,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D48" s="10">
         <v>3</v>
@@ -1836,13 +1860,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D49" s="10">
         <v>3</v>
@@ -1854,13 +1878,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D50" s="6">
         <v>4</v>
@@ -1872,13 +1896,13 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D51" s="10">
         <v>4</v>
@@ -1890,13 +1914,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D52" s="10">
         <v>4</v>
@@ -1908,13 +1932,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D53" s="10">
         <v>4</v>
@@ -1926,13 +1950,13 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D54" s="10">
         <v>4</v>
@@ -1944,13 +1968,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D55" s="10">
         <v>4</v>
@@ -1962,13 +1986,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D56" s="10">
         <v>4</v>
@@ -1980,13 +2004,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D57" s="10">
         <v>4</v>
@@ -1998,13 +2022,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D58" s="10">
         <v>4</v>
@@ -2016,13 +2040,13 @@
     </row>
     <row r="59" spans="1:5" ht="29">
       <c r="A59" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D59" s="10">
         <v>4</v>
@@ -2034,13 +2058,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D60" s="10">
         <v>4</v>
@@ -2052,13 +2076,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D61" s="10">
         <v>4</v>
@@ -2070,13 +2094,13 @@
     </row>
     <row r="62" spans="1:5" ht="29">
       <c r="A62" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D62" s="10">
         <v>4</v>
@@ -2088,13 +2112,13 @@
     </row>
     <row r="63" spans="1:5" ht="29">
       <c r="A63" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D63" s="10">
         <v>4</v>
@@ -2106,13 +2130,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D64" s="6">
         <v>5</v>
@@ -2124,13 +2148,13 @@
     </row>
     <row r="65" spans="1:5" ht="29">
       <c r="A65" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D65" s="6">
         <v>5</v>
@@ -2142,13 +2166,13 @@
     </row>
     <row r="66" spans="1:5" ht="29">
       <c r="A66" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D66" s="6">
         <v>5</v>

</xml_diff>

<commit_message>
Improved profile code uniqueness
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="136">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -111,9 +111,6 @@
     <t>PEPPOL Invoice profile V2</t>
   </si>
   <si>
-    <t>PEPPOL Catalogue profile V1</t>
-  </si>
-  <si>
     <t>1.2.0</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:Catalogue-2::Catalogue##urn:www.cenbii.eu:transaction:biitrns019:ver2.0:extended:urn:www.peppol.eu:bis:peppol1a:ver4.0::2.1</t>
   </si>
   <si>
-    <t>PEPPOL Billing profile V1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:www.cenbii.eu:transaction:biitrns010:ver2.0:extended:urn:www.peppol.eu:bis:peppol5a:ver2.0::2.1</t>
   </si>
   <si>
@@ -225,12 +219,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.1::2.1</t>
   </si>
   <si>
-    <t>XRechnung Invoice V1.1</t>
-  </si>
-  <si>
-    <t>XRechnung CreditNote V1.1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.1::2.1</t>
   </si>
   <si>
@@ -424,6 +412,27 @@
   </si>
   <si>
     <t>PEPPOL Procurement profile CreditNote V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Catalogue profile Catalogue V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Billing profile Invoice V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Billing profile CreditNote V1</t>
+  </si>
+  <si>
+    <t>PEPPOL Catalogue profile ApplicationResponse V1</t>
+  </si>
+  <si>
+    <t>XRechnung UBL Invoice V1.1</t>
+  </si>
+  <si>
+    <t>XRechnung UBL CreditNote V1.1</t>
+  </si>
+  <si>
+    <t>XRechnung CII Invoice V1.1</t>
   </si>
 </sst>
 </file>
@@ -923,8 +932,8 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A2:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -941,22 +950,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="29">
@@ -964,7 +973,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -985,12 +994,12 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="6" t="b">
@@ -1006,12 +1015,12 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="6" t="b">
@@ -1024,15 +1033,15 @@
     </row>
     <row r="5" spans="1:7" ht="29">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="6" t="b">
@@ -1045,10 +1054,10 @@
     </row>
     <row r="6" spans="1:7" ht="29">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>132</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1066,10 +1075,10 @@
     </row>
     <row r="7" spans="1:7" ht="29">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>132</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -1087,16 +1096,16 @@
     </row>
     <row r="8" spans="1:7" ht="29">
       <c r="A8" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="6" t="b">
         <f>FALSE</f>
@@ -1105,15 +1114,15 @@
     </row>
     <row r="9" spans="1:7" ht="29">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="6" t="b">
@@ -1126,16 +1135,16 @@
     </row>
     <row r="10" spans="1:7" ht="29">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="10" t="b">
         <f>TRUE</f>
@@ -1145,18 +1154,18 @@
         <v>3</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" ht="29">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" s="8">
         <v>3</v>
@@ -1171,12 +1180,12 @@
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="6" t="b">
@@ -1192,13 +1201,13 @@
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="6" t="b">
         <f>FALSE</f>
@@ -1207,10 +1216,10 @@
     </row>
     <row r="14" spans="1:7" ht="29">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
@@ -1228,10 +1237,10 @@
     </row>
     <row r="15" spans="1:7" ht="29">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>20</v>
@@ -1249,10 +1258,10 @@
     </row>
     <row r="16" spans="1:7" ht="29">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
@@ -1270,16 +1279,16 @@
     </row>
     <row r="17" spans="1:7" ht="29">
       <c r="A17" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="6" t="b">
         <f>FALSE</f>
@@ -1288,16 +1297,16 @@
     </row>
     <row r="18" spans="1:7" ht="29">
       <c r="A18" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="6" t="b">
         <f>FALSE</f>
@@ -1306,15 +1315,15 @@
     </row>
     <row r="19" spans="1:7" ht="29">
       <c r="A19" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="6" t="b">
@@ -1324,10 +1333,10 @@
     </row>
     <row r="20" spans="1:7" ht="29">
       <c r="A20" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1342,10 +1351,10 @@
     </row>
     <row r="21" spans="1:7" ht="29">
       <c r="A21" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
@@ -1360,10 +1369,10 @@
     </row>
     <row r="22" spans="1:7" ht="29">
       <c r="A22" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1378,15 +1387,15 @@
     </row>
     <row r="23" spans="1:7" ht="29">
       <c r="A23" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="6" t="b">
@@ -1396,10 +1405,10 @@
     </row>
     <row r="24" spans="1:7" ht="29">
       <c r="A24" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1414,10 +1423,10 @@
     </row>
     <row r="25" spans="1:7" ht="29">
       <c r="A25" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>23</v>
@@ -1435,10 +1444,10 @@
     </row>
     <row r="26" spans="1:7" ht="43.5">
       <c r="A26" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>25</v>
@@ -1453,16 +1462,16 @@
     </row>
     <row r="27" spans="1:7" ht="29">
       <c r="A27" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E27" s="6" t="b">
         <f>FALSE</f>
@@ -1471,16 +1480,16 @@
     </row>
     <row r="28" spans="1:7" ht="29">
       <c r="A28" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" s="6" t="b">
         <v>1</v>
@@ -1489,18 +1498,18 @@
         <v>3</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="29">
       <c r="A29" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D29" s="8">
         <v>3</v>
@@ -1512,16 +1521,16 @@
     </row>
     <row r="30" spans="1:7" ht="29">
       <c r="A30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D30" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="6" t="b">
         <f>FALSE</f>
@@ -1529,17 +1538,17 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="29">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="D31" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="6" t="b">
         <f>FALSE</f>
@@ -1548,15 +1557,15 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="6">
+        <v>46</v>
+      </c>
+      <c r="D32" s="10">
         <v>2</v>
       </c>
       <c r="E32" s="6" t="b">
@@ -1566,15 +1575,15 @@
     </row>
     <row r="33" spans="1:6" ht="29">
       <c r="A33" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="6">
+        <v>47</v>
+      </c>
+      <c r="D33" s="10">
         <v>2</v>
       </c>
       <c r="E33" s="6" t="b">
@@ -1584,13 +1593,13 @@
     </row>
     <row r="34" spans="1:6" ht="43.5">
       <c r="A34" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D34" s="8">
         <v>3</v>
@@ -1602,13 +1611,13 @@
     </row>
     <row r="35" spans="1:6" ht="43.5">
       <c r="A35" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D35" s="8">
         <v>3</v>
@@ -1620,15 +1629,15 @@
     </row>
     <row r="36" spans="1:6" ht="29">
       <c r="A36" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="6">
+        <v>52</v>
+      </c>
+      <c r="D36" s="10">
         <v>3</v>
       </c>
       <c r="E36" s="6" t="b">
@@ -1638,15 +1647,15 @@
     </row>
     <row r="37" spans="1:6" ht="29">
       <c r="A37" s="10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="6">
+        <v>53</v>
+      </c>
+      <c r="D37" s="10">
         <v>3</v>
       </c>
       <c r="E37" s="10" t="b">
@@ -1656,15 +1665,15 @@
     </row>
     <row r="38" spans="1:6" ht="29">
       <c r="A38" s="10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="6">
+        <v>54</v>
+      </c>
+      <c r="D38" s="10">
         <v>3</v>
       </c>
       <c r="E38" s="10" t="b">
@@ -1674,13 +1683,13 @@
     </row>
     <row r="39" spans="1:6" ht="29">
       <c r="A39" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D39" s="6">
         <v>3</v>
@@ -1692,13 +1701,13 @@
     </row>
     <row r="40" spans="1:6" ht="29">
       <c r="A40" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D40" s="6">
         <v>3</v>
@@ -1710,13 +1719,13 @@
     </row>
     <row r="41" spans="1:6" ht="29">
       <c r="A41" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D41" s="6">
         <v>3</v>
@@ -1728,13 +1737,13 @@
     </row>
     <row r="42" spans="1:6" ht="29">
       <c r="A42" s="10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D42" s="6">
         <v>3</v>
@@ -1746,13 +1755,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D43" s="10">
         <v>3</v>
@@ -1766,13 +1775,13 @@
     </row>
     <row r="44" spans="1:6" ht="29">
       <c r="A44" s="4" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D44" s="10">
         <v>3</v>
@@ -1786,13 +1795,13 @@
     </row>
     <row r="45" spans="1:6" ht="29">
       <c r="A45" s="4" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D45" s="10">
         <v>3</v>
@@ -1806,13 +1815,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D46" s="10">
         <v>3</v>
@@ -1824,13 +1833,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D47" s="10">
         <v>3</v>
@@ -1842,13 +1851,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D48" s="10">
         <v>3</v>
@@ -1860,13 +1869,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D49" s="10">
         <v>3</v>
@@ -1878,13 +1887,13 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D50" s="6">
         <v>4</v>
@@ -1896,13 +1905,13 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D51" s="10">
         <v>4</v>
@@ -1914,13 +1923,13 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D52" s="10">
         <v>4</v>
@@ -1932,13 +1941,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D53" s="10">
         <v>4</v>
@@ -1950,13 +1959,13 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D54" s="10">
         <v>4</v>
@@ -1968,13 +1977,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D55" s="10">
         <v>4</v>
@@ -1986,13 +1995,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D56" s="10">
         <v>4</v>
@@ -2004,13 +2013,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D57" s="10">
         <v>4</v>
@@ -2022,13 +2031,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D58" s="10">
         <v>4</v>
@@ -2038,15 +2047,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="29">
+    <row r="59" spans="1:5">
       <c r="A59" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D59" s="10">
         <v>4</v>
@@ -2058,13 +2067,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D60" s="10">
         <v>4</v>
@@ -2076,13 +2085,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D61" s="10">
         <v>4</v>
@@ -2094,13 +2103,13 @@
     </row>
     <row r="62" spans="1:5" ht="29">
       <c r="A62" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D62" s="10">
         <v>4</v>
@@ -2112,13 +2121,13 @@
     </row>
     <row r="63" spans="1:5" ht="29">
       <c r="A63" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D63" s="10">
         <v>4</v>
@@ -2130,13 +2139,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D64" s="6">
         <v>5</v>
@@ -2148,13 +2157,13 @@
     </row>
     <row r="65" spans="1:5" ht="29">
       <c r="A65" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D65" s="6">
         <v>5</v>
@@ -2166,13 +2175,13 @@
     </row>
     <row r="66" spans="1:5" ht="29">
       <c r="A66" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D66" s="6">
         <v>5</v>
@@ -2186,8 +2195,5 @@
   <autoFilter ref="A1:F66"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="D14:D16" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Polish document type and process identifiers
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="142">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -433,6 +433,24 @@
   </si>
   <si>
     <t>XRechnung CII Invoice V1.1</t>
+  </si>
+  <si>
+    <t>PEF.PL Accounting Note v1</t>
+  </si>
+  <si>
+    <t>PEF.PL Correcting Invoice v1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:billing:3.0#extended#urn:fdc:www.efaktura.gov.pl:ver1.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:ReceiptAdvice-2::ReceiptAdvice##urn:fdc:www.efaktura.gov.pl:ver1.0:trns:receipt_advice:ver1.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:fdc:www.efaktura.gov.pl:ver1.0:trns:account_corr:ver1.0::2.1</t>
+  </si>
+  <si>
+    <t>PEF.PL Receipt Advice v1</t>
   </si>
 </sst>
 </file>
@@ -929,23 +947,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A2:A66"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="129.26953125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="129.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.453125" style="6"/>
+    <col min="5" max="5" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -968,7 +986,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -989,7 +1007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29">
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1010,7 +1028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1031,7 +1049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="4" t="s">
         <v>129</v>
       </c>
@@ -1052,7 +1070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="4" t="s">
         <v>132</v>
       </c>
@@ -1073,7 +1091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="4" t="s">
         <v>132</v>
       </c>
@@ -1094,7 +1112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29">
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
@@ -1112,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1133,7 +1151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29">
+    <row r="10" spans="1:7" ht="30">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1157,7 +1175,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" ht="29">
+    <row r="11" spans="1:7" s="10" customFormat="1" ht="30">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1175,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1196,7 +1214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1214,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29">
+    <row r="14" spans="1:7" ht="30">
       <c r="A14" s="2" t="s">
         <v>130</v>
       </c>
@@ -1235,7 +1253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="29">
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="2" t="s">
         <v>131</v>
       </c>
@@ -1256,7 +1274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29">
+    <row r="16" spans="1:7" ht="30">
       <c r="A16" s="2" t="s">
         <v>130</v>
       </c>
@@ -1277,7 +1295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29">
+    <row r="17" spans="1:7" ht="30">
       <c r="A17" s="2" t="s">
         <v>113</v>
       </c>
@@ -1295,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="29">
+    <row r="18" spans="1:7" ht="30">
       <c r="A18" s="2" t="s">
         <v>114</v>
       </c>
@@ -1313,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="29">
+    <row r="19" spans="1:7" ht="30">
       <c r="A19" s="4" t="s">
         <v>125</v>
       </c>
@@ -1331,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29">
+    <row r="20" spans="1:7" ht="30">
       <c r="A20" s="4" t="s">
         <v>126</v>
       </c>
@@ -1349,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="29">
+    <row r="21" spans="1:7" ht="30">
       <c r="A21" s="4" t="s">
         <v>126</v>
       </c>
@@ -1367,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="29">
+    <row r="22" spans="1:7" ht="30">
       <c r="A22" s="4" t="s">
         <v>127</v>
       </c>
@@ -1385,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="29">
+    <row r="23" spans="1:7" ht="30">
       <c r="A23" s="4" t="s">
         <v>128</v>
       </c>
@@ -1403,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29">
+    <row r="24" spans="1:7" ht="30">
       <c r="A24" s="4" t="s">
         <v>127</v>
       </c>
@@ -1421,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="29">
+    <row r="25" spans="1:7" ht="45">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -1442,7 +1460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="43.5">
+    <row r="26" spans="1:7" ht="45">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -1460,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="29">
+    <row r="27" spans="1:7" ht="30">
       <c r="A27" s="4" t="s">
         <v>123</v>
       </c>
@@ -1478,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="29">
+    <row r="28" spans="1:7" ht="30">
       <c r="A28" s="4" t="s">
         <v>124</v>
       </c>
@@ -1501,7 +1519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="29">
+    <row r="29" spans="1:7" ht="30">
       <c r="A29" s="4" t="s">
         <v>124</v>
       </c>
@@ -1519,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="29">
+    <row r="30" spans="1:7" ht="30">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
@@ -1537,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="29">
+    <row r="31" spans="1:7" ht="30">
       <c r="A31" s="10" t="s">
         <v>41</v>
       </c>
@@ -1555,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="30">
       <c r="A32" s="4" t="s">
         <v>110</v>
       </c>
@@ -1573,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="29">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="4" t="s">
         <v>111</v>
       </c>
@@ -1591,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="43.5">
+    <row r="34" spans="1:6" ht="45">
       <c r="A34" s="4" t="s">
         <v>122</v>
       </c>
@@ -1609,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="43.5">
+    <row r="35" spans="1:6" ht="45">
       <c r="A35" s="4" t="s">
         <v>121</v>
       </c>
@@ -1627,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="29">
+    <row r="36" spans="1:6" ht="30">
       <c r="A36" s="4" t="s">
         <v>112</v>
       </c>
@@ -1645,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="29">
+    <row r="37" spans="1:6" ht="30">
       <c r="A37" s="10" t="s">
         <v>120</v>
       </c>
@@ -1663,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="29">
+    <row r="38" spans="1:6" ht="30">
       <c r="A38" s="10" t="s">
         <v>119</v>
       </c>
@@ -1681,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="29">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="10" t="s">
         <v>118</v>
       </c>
@@ -1699,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="29">
+    <row r="40" spans="1:6" ht="30">
       <c r="A40" s="10" t="s">
         <v>117</v>
       </c>
@@ -1717,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="29">
+    <row r="41" spans="1:6" ht="30">
       <c r="A41" s="10" t="s">
         <v>115</v>
       </c>
@@ -1735,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="29">
+    <row r="42" spans="1:6" ht="30">
       <c r="A42" s="10" t="s">
         <v>116</v>
       </c>
@@ -1753,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="4" t="s">
         <v>133</v>
       </c>
@@ -1773,7 +1791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="29">
+    <row r="44" spans="1:6" ht="30">
       <c r="A44" s="4" t="s">
         <v>134</v>
       </c>
@@ -1793,7 +1811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="29">
+    <row r="45" spans="1:6" ht="30">
       <c r="A45" s="4" t="s">
         <v>135</v>
       </c>
@@ -1867,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="4" t="s">
         <v>70</v>
       </c>
@@ -1885,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" ht="30">
       <c r="A50" s="4" t="s">
         <v>77</v>
       </c>
@@ -1921,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" ht="30">
       <c r="A52" s="4" t="s">
         <v>88</v>
       </c>
@@ -1957,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" ht="30">
       <c r="A54" s="4" t="s">
         <v>90</v>
       </c>
@@ -2101,7 +2119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="29">
+    <row r="62" spans="1:5" ht="30">
       <c r="A62" t="s">
         <v>100</v>
       </c>
@@ -2119,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="29">
+    <row r="63" spans="1:5" ht="30">
       <c r="A63" s="4" t="s">
         <v>101</v>
       </c>
@@ -2137,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" ht="30">
       <c r="A64" s="4" t="s">
         <v>104</v>
       </c>
@@ -2155,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="29">
+    <row r="65" spans="1:5" ht="30">
       <c r="A65" s="4" t="s">
         <v>105</v>
       </c>
@@ -2173,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="29">
+    <row r="66" spans="1:5" ht="30">
       <c r="A66" s="4" t="s">
         <v>106</v>
       </c>
@@ -2187,6 +2205,60 @@
         <v>5</v>
       </c>
       <c r="E66" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D67" s="6">
+        <v>6</v>
+      </c>
+      <c r="E67" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="45">
+      <c r="A68" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" s="10">
+        <v>6</v>
+      </c>
+      <c r="E68" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="30">
+      <c r="A69" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" s="10">
+        <v>6</v>
+      </c>
+      <c r="E69" s="10" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added new columns: "Issued by OpenPEPPOL", "BIS version" and "Domain Community"
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$F$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$J$69</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="148">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -451,6 +451,24 @@
   </si>
   <si>
     <t>PEF.PL Receipt Advice v1</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>BIS version</t>
+  </si>
+  <si>
+    <t>Domain Community</t>
+  </si>
+  <si>
+    <t>PRAC</t>
+  </si>
+  <si>
+    <t>POAC</t>
+  </si>
+  <si>
+    <t>Issued OpenPEPPOL?</t>
   </si>
 </sst>
 </file>
@@ -516,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -533,20 +551,14 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,26 +959,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G69"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="47.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="129.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="6"/>
+    <col min="2" max="2" width="19" style="4" customWidth="1"/>
+    <col min="3" max="3" width="103.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="30">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -979,14 +993,26 @@
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30">
+      <c r="G1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -996,18 +1022,28 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="E2" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30">
+      <c r="H2" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="45">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1017,18 +1053,28 @@
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E3" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30">
+      <c r="H3" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1038,18 +1084,28 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30">
+      <c r="H4" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45">
       <c r="A5" s="4" t="s">
         <v>129</v>
       </c>
@@ -1059,18 +1115,28 @@
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="E5" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30">
+      <c r="H5" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45">
       <c r="A6" s="4" t="s">
         <v>132</v>
       </c>
@@ -1080,18 +1146,28 @@
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="E6" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30">
+      <c r="H6" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45">
       <c r="A7" s="4" t="s">
         <v>132</v>
       </c>
@@ -1101,18 +1177,28 @@
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="E7" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
+      <c r="H7" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45">
       <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
@@ -1122,15 +1208,25 @@
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
+      <c r="E8" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" hidden="1">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1140,18 +1236,28 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="E9" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="30">
+      <c r="H9" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" hidden="1">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1161,21 +1267,31 @@
       <c r="C10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="10" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>3</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="E10" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="H10" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" hidden="1">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1185,15 +1301,25 @@
       <c r="C11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="8">
-        <v>3</v>
-      </c>
-      <c r="E11" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30">
+      <c r="D11" s="6">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" hidden="1">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1203,18 +1329,28 @@
       <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="E12" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="30">
+      <c r="H12" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" hidden="1">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1224,15 +1360,25 @@
       <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30">
+      <c r="E13" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" hidden="1">
       <c r="A14" s="2" t="s">
         <v>130</v>
       </c>
@@ -1242,18 +1388,28 @@
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="E14" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="30">
+      <c r="H14" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" hidden="1">
       <c r="A15" s="2" t="s">
         <v>131</v>
       </c>
@@ -1263,18 +1419,28 @@
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="E15" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="30">
+      <c r="H15" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" hidden="1">
       <c r="A16" s="2" t="s">
         <v>130</v>
       </c>
@@ -1284,18 +1450,28 @@
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="E16" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="30">
+      <c r="H16" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" hidden="1">
       <c r="A17" s="2" t="s">
         <v>113</v>
       </c>
@@ -1305,15 +1481,25 @@
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30">
+      <c r="E17" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" hidden="1">
       <c r="A18" s="2" t="s">
         <v>114</v>
       </c>
@@ -1323,15 +1509,25 @@
       <c r="C18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30">
+      <c r="E18" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="4">
+        <v>2</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" hidden="1">
       <c r="A19" s="4" t="s">
         <v>125</v>
       </c>
@@ -1341,15 +1537,25 @@
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30">
+      <c r="E19" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" hidden="1">
       <c r="A20" s="4" t="s">
         <v>126</v>
       </c>
@@ -1359,15 +1565,25 @@
       <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30">
+      <c r="E20" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" hidden="1">
       <c r="A21" s="4" t="s">
         <v>126</v>
       </c>
@@ -1377,15 +1593,25 @@
       <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30">
+      <c r="E21" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" hidden="1">
       <c r="A22" s="4" t="s">
         <v>127</v>
       </c>
@@ -1395,15 +1621,25 @@
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30">
+      <c r="E22" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" hidden="1">
       <c r="A23" s="4" t="s">
         <v>128</v>
       </c>
@@ -1413,15 +1649,25 @@
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30">
+      <c r="E23" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" hidden="1">
       <c r="A24" s="4" t="s">
         <v>127</v>
       </c>
@@ -1431,15 +1677,25 @@
       <c r="C24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45">
+      <c r="E24" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I24" s="4">
+        <v>1</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" hidden="1">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -1449,18 +1705,25 @@
       <c r="C25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="E25" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="45">
+      <c r="H25" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="45" hidden="1">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -1470,15 +1733,22 @@
       <c r="C26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30">
+      <c r="E26" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="45" hidden="1">
       <c r="A27" s="4" t="s">
         <v>123</v>
       </c>
@@ -1488,15 +1758,25 @@
       <c r="C27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30">
+      <c r="E27" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I27" s="4">
+        <v>1</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" hidden="1">
       <c r="A28" s="4" t="s">
         <v>124</v>
       </c>
@@ -1506,20 +1786,30 @@
       <c r="C28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="6">
-        <v>3</v>
-      </c>
-      <c r="G28" s="6" t="s">
+      <c r="E28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="30">
+      <c r="H28" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45" hidden="1">
       <c r="A29" s="4" t="s">
         <v>124</v>
       </c>
@@ -1529,15 +1819,25 @@
       <c r="C29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="8">
-        <v>3</v>
-      </c>
-      <c r="E29" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30">
+      <c r="D29" s="6">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" hidden="1">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
@@ -1547,16 +1847,26 @@
       <c r="C30" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30">
-      <c r="A31" s="10" t="s">
+      <c r="E30" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" hidden="1">
+      <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1565,15 +1875,25 @@
       <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30">
+      <c r="E31" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" hidden="1">
       <c r="A32" s="4" t="s">
         <v>110</v>
       </c>
@@ -1583,15 +1903,25 @@
       <c r="C32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="4">
         <v>2</v>
       </c>
-      <c r="E32" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30">
+      <c r="E32" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I32" s="4">
+        <v>3</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30" hidden="1">
       <c r="A33" s="4" t="s">
         <v>111</v>
       </c>
@@ -1601,15 +1931,25 @@
       <c r="C33" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="4">
         <v>2</v>
       </c>
-      <c r="E33" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45">
+      <c r="E33" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="4">
+        <v>3</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="45" hidden="1">
       <c r="A34" s="4" t="s">
         <v>122</v>
       </c>
@@ -1619,15 +1959,22 @@
       <c r="C34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="8">
-        <v>3</v>
-      </c>
-      <c r="E34" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45">
+      <c r="D34" s="6">
+        <v>3</v>
+      </c>
+      <c r="E34" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="45" hidden="1">
       <c r="A35" s="4" t="s">
         <v>121</v>
       </c>
@@ -1637,15 +1984,22 @@
       <c r="C35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="8">
-        <v>3</v>
-      </c>
-      <c r="E35" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30">
+      <c r="D35" s="6">
+        <v>3</v>
+      </c>
+      <c r="E35" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30" hidden="1">
       <c r="A36" s="4" t="s">
         <v>112</v>
       </c>
@@ -1655,16 +2009,26 @@
       <c r="C36" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="10">
-        <v>3</v>
-      </c>
-      <c r="E36" s="6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30">
-      <c r="A37" s="10" t="s">
+      <c r="D36" s="4">
+        <v>3</v>
+      </c>
+      <c r="E36" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I36" s="4">
+        <v>3</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="45">
+      <c r="A37" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1673,16 +2037,26 @@
       <c r="C37" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="10">
-        <v>3</v>
-      </c>
-      <c r="E37" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30">
-      <c r="A38" s="10" t="s">
+      <c r="D37" s="4">
+        <v>3</v>
+      </c>
+      <c r="E37" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I37" s="4">
+        <v>1</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="45">
+      <c r="A38" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1691,16 +2065,26 @@
       <c r="C38" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="10">
-        <v>3</v>
-      </c>
-      <c r="E38" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30">
-      <c r="A39" s="10" t="s">
+      <c r="D38" s="4">
+        <v>3</v>
+      </c>
+      <c r="E38" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I38" s="4">
+        <v>1</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="45">
+      <c r="A39" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1709,16 +2093,26 @@
       <c r="C39" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="6">
-        <v>3</v>
-      </c>
-      <c r="E39" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="30">
-      <c r="A40" s="10" t="s">
+      <c r="D39" s="4">
+        <v>3</v>
+      </c>
+      <c r="E39" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="45">
+      <c r="A40" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1727,16 +2121,26 @@
       <c r="C40" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="6">
-        <v>3</v>
-      </c>
-      <c r="E40" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30">
-      <c r="A41" s="10" t="s">
+      <c r="D40" s="4">
+        <v>3</v>
+      </c>
+      <c r="E40" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I40" s="4">
+        <v>1</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="45">
+      <c r="A41" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1745,16 +2149,26 @@
       <c r="C41" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="6">
-        <v>3</v>
-      </c>
-      <c r="E41" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="30">
-      <c r="A42" s="10" t="s">
+      <c r="D41" s="4">
+        <v>3</v>
+      </c>
+      <c r="E41" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I41" s="4">
+        <v>1</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="45">
+      <c r="A42" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1763,15 +2177,25 @@
       <c r="C42" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="6">
-        <v>3</v>
-      </c>
-      <c r="E42" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30">
+      <c r="D42" s="4">
+        <v>3</v>
+      </c>
+      <c r="E42" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I42" s="4">
+        <v>1</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="30" hidden="1">
       <c r="A43" s="4" t="s">
         <v>133</v>
       </c>
@@ -1781,17 +2205,24 @@
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="10">
-        <v>3</v>
-      </c>
-      <c r="E43" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" s="6">
+      <c r="D43" s="4">
+        <v>3</v>
+      </c>
+      <c r="E43" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="30">
+      <c r="H43" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="30" hidden="1">
       <c r="A44" s="4" t="s">
         <v>134</v>
       </c>
@@ -1801,17 +2232,24 @@
       <c r="C44" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="10">
-        <v>3</v>
-      </c>
-      <c r="E44" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="6">
+      <c r="D44" s="4">
+        <v>3</v>
+      </c>
+      <c r="E44" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="30">
+      <c r="H44" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="30" hidden="1">
       <c r="A45" s="4" t="s">
         <v>135</v>
       </c>
@@ -1821,17 +2259,24 @@
       <c r="C45" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="10">
-        <v>3</v>
-      </c>
-      <c r="E45" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" s="6">
+      <c r="D45" s="4">
+        <v>3</v>
+      </c>
+      <c r="E45" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="H45" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" hidden="1">
       <c r="A46" s="4" t="s">
         <v>67</v>
       </c>
@@ -1841,15 +2286,22 @@
       <c r="C46" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D46" s="10">
-        <v>3</v>
-      </c>
-      <c r="E46" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="D46" s="4">
+        <v>3</v>
+      </c>
+      <c r="E46" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" hidden="1">
       <c r="A47" s="4" t="s">
         <v>68</v>
       </c>
@@ -1859,15 +2311,22 @@
       <c r="C47" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D47" s="10">
-        <v>3</v>
-      </c>
-      <c r="E47" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="D47" s="4">
+        <v>3</v>
+      </c>
+      <c r="E47" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="30" hidden="1">
       <c r="A48" s="4" t="s">
         <v>69</v>
       </c>
@@ -1877,15 +2336,22 @@
       <c r="C48" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="10">
-        <v>3</v>
-      </c>
-      <c r="E48" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30">
+      <c r="D48" s="4">
+        <v>3</v>
+      </c>
+      <c r="E48" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="30" hidden="1">
       <c r="A49" s="4" t="s">
         <v>70</v>
       </c>
@@ -1895,15 +2361,22 @@
       <c r="C49" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="10">
-        <v>3</v>
-      </c>
-      <c r="E49" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30">
+      <c r="D49" s="4">
+        <v>3</v>
+      </c>
+      <c r="E49" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H49" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="30" hidden="1">
       <c r="A50" s="4" t="s">
         <v>77</v>
       </c>
@@ -1913,15 +2386,25 @@
       <c r="C50" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="4">
         <v>4</v>
       </c>
-      <c r="E50" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="E50" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I50" s="4">
+        <v>1</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="30" hidden="1">
       <c r="A51" s="4" t="s">
         <v>87</v>
       </c>
@@ -1931,15 +2414,25 @@
       <c r="C51" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="4">
         <v>4</v>
       </c>
-      <c r="E51" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30">
+      <c r="E51" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I51" s="4">
+        <v>3</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="30" hidden="1">
       <c r="A52" s="4" t="s">
         <v>88</v>
       </c>
@@ -1949,15 +2442,25 @@
       <c r="C52" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="4">
         <v>4</v>
       </c>
-      <c r="E52" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="E52" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I52" s="4">
+        <v>3</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" hidden="1">
       <c r="A53" s="4" t="s">
         <v>89</v>
       </c>
@@ -1967,15 +2470,25 @@
       <c r="C53" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="4">
         <v>4</v>
       </c>
-      <c r="E53" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30">
+      <c r="E53" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I53" s="4">
+        <v>3</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30" hidden="1">
       <c r="A54" s="4" t="s">
         <v>90</v>
       </c>
@@ -1985,15 +2498,25 @@
       <c r="C54" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="4">
         <v>4</v>
       </c>
-      <c r="E54" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="E54" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I54" s="4">
+        <v>3</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="30" hidden="1">
       <c r="A55" s="4" t="s">
         <v>91</v>
       </c>
@@ -2003,15 +2526,25 @@
       <c r="C55" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D55" s="4">
         <v>4</v>
       </c>
-      <c r="E55" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="E55" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I55" s="4">
+        <v>3</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="30" hidden="1">
       <c r="A56" s="4" t="s">
         <v>92</v>
       </c>
@@ -2021,15 +2554,25 @@
       <c r="C56" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D56" s="4">
         <v>4</v>
       </c>
-      <c r="E56" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="E56" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I56" s="4">
+        <v>3</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="30" hidden="1">
       <c r="A57" s="4" t="s">
         <v>93</v>
       </c>
@@ -2039,15 +2582,25 @@
       <c r="C57" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D57" s="4">
         <v>4</v>
       </c>
-      <c r="E57" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="E57" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I57" s="4">
+        <v>3</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="30" hidden="1">
       <c r="A58" s="4" t="s">
         <v>94</v>
       </c>
@@ -2057,15 +2610,25 @@
       <c r="C58" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="4">
         <v>4</v>
       </c>
-      <c r="E58" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="E58" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H58" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I58" s="4">
+        <v>3</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="30" hidden="1">
       <c r="A59" s="4" t="s">
         <v>95</v>
       </c>
@@ -2075,15 +2638,25 @@
       <c r="C59" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="4">
         <v>4</v>
       </c>
-      <c r="E59" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="E59" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H59" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I59" s="4">
+        <v>3</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="30" hidden="1">
       <c r="A60" s="4" t="s">
         <v>96</v>
       </c>
@@ -2093,15 +2666,22 @@
       <c r="C60" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D60" s="4">
         <v>4</v>
       </c>
-      <c r="E60" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="E60" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H60" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="30" hidden="1">
       <c r="A61" s="4" t="s">
         <v>98</v>
       </c>
@@ -2111,16 +2691,23 @@
       <c r="C61" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D61" s="4">
         <v>4</v>
       </c>
-      <c r="E61" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30">
-      <c r="A62" t="s">
+      <c r="E61" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="30" hidden="1">
+      <c r="A62" s="8" t="s">
         <v>100</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -2129,15 +2716,25 @@
       <c r="C62" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D62" s="10">
+      <c r="D62" s="4">
         <v>4</v>
       </c>
-      <c r="E62" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="30">
+      <c r="E62" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I62" s="4">
+        <v>3</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="45" hidden="1">
       <c r="A63" s="4" t="s">
         <v>101</v>
       </c>
@@ -2147,15 +2744,25 @@
       <c r="C63" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="4">
         <v>4</v>
       </c>
-      <c r="E63" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="30">
+      <c r="E63" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H63" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I63" s="4">
+        <v>3</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="30" hidden="1">
       <c r="A64" s="4" t="s">
         <v>104</v>
       </c>
@@ -2165,15 +2772,22 @@
       <c r="C64" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64" s="4">
         <v>5</v>
       </c>
-      <c r="E64" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30">
+      <c r="E64" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H64" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="30" hidden="1">
       <c r="A65" s="4" t="s">
         <v>105</v>
       </c>
@@ -2183,15 +2797,22 @@
       <c r="C65" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D65" s="4">
         <v>5</v>
       </c>
-      <c r="E65" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30">
+      <c r="E65" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H65" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="30" hidden="1">
       <c r="A66" s="4" t="s">
         <v>106</v>
       </c>
@@ -2201,15 +2822,22 @@
       <c r="C66" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66" s="4">
         <v>5</v>
       </c>
-      <c r="E66" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="E66" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H66" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="30" hidden="1">
       <c r="A67" s="4" t="s">
         <v>136</v>
       </c>
@@ -2219,15 +2847,22 @@
       <c r="C67" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D67" s="4">
         <v>6</v>
       </c>
-      <c r="E67" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="45">
+      <c r="E67" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="45" hidden="1">
       <c r="A68" s="4" t="s">
         <v>137</v>
       </c>
@@ -2237,15 +2872,22 @@
       <c r="C68" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="4">
         <v>6</v>
       </c>
-      <c r="E68" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="30">
+      <c r="E68" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H68" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30" hidden="1">
       <c r="A69" s="4" t="s">
         <v>141</v>
       </c>
@@ -2255,16 +2897,29 @@
       <c r="C69" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="4">
         <v>6</v>
       </c>
-      <c r="E69" s="10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="E69" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H69" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F66"/>
+  <autoFilter ref="A1:J69">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="PRAC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added TICC-102 document types
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="156">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -469,6 +469,30 @@
   </si>
   <si>
     <t>Issued OpenPEPPOL?</t>
+  </si>
+  <si>
+    <t>AU-NZ Self-Billing 3.0 Invoice</t>
+  </si>
+  <si>
+    <t>AU-NZ PEPPOL BIS Billing 3.0 CreditNote</t>
+  </si>
+  <si>
+    <t>AU-NZ PEPPOL BIS Billing 3.0 Invoice</t>
+  </si>
+  <si>
+    <t>AU-NZ Self-Billing 3.0 CreditNote</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#conformant#urn:fdc:peppol.eu:2017:poacc:billing:international:aunz:3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#conformant#urn:fdc:peppol.eu:2017:poacc:selfbilling:international:aunz:3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:fdc:peppol.eu:2017:poacc:billing:international:aunz:3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:fdc:peppol.eu:2017:poacc:selfbilling:international:aunz:3.0::2.1</t>
   </si>
 </sst>
 </file>
@@ -959,28 +983,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.59765625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="4" customWidth="1"/>
-    <col min="3" max="3" width="103.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="103.1328125" style="4" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="4"/>
+    <col min="5" max="5" width="14.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.73046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.3984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.5">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -1012,7 +1035,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45">
+    <row r="2" spans="1:10" ht="42.75">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1043,7 +1066,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45">
+    <row r="3" spans="1:10" ht="42.75">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1074,7 +1097,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45">
+    <row r="4" spans="1:10" ht="28.5">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1105,7 +1128,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="45">
+    <row r="5" spans="1:10" ht="28.5">
       <c r="A5" s="4" t="s">
         <v>129</v>
       </c>
@@ -1136,7 +1159,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45">
+    <row r="6" spans="1:10" ht="28.5">
       <c r="A6" s="4" t="s">
         <v>132</v>
       </c>
@@ -1167,7 +1190,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45">
+    <row r="7" spans="1:10" ht="28.5">
       <c r="A7" s="4" t="s">
         <v>132</v>
       </c>
@@ -1198,7 +1221,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45">
+    <row r="8" spans="1:10" ht="28.5">
       <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
@@ -1226,7 +1249,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30" hidden="1">
+    <row r="9" spans="1:10" ht="28.5">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1257,7 +1280,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="45" hidden="1">
+    <row r="10" spans="1:10" ht="28.5">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1291,7 +1314,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45" hidden="1">
+    <row r="11" spans="1:10" ht="28.5">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1319,7 +1342,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" hidden="1">
+    <row r="12" spans="1:10" ht="28.5">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1350,7 +1373,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" hidden="1">
+    <row r="13" spans="1:10" ht="28.5">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1378,7 +1401,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" hidden="1">
+    <row r="14" spans="1:10" ht="28.5">
       <c r="A14" s="2" t="s">
         <v>130</v>
       </c>
@@ -1409,7 +1432,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45" hidden="1">
+    <row r="15" spans="1:10" ht="28.5">
       <c r="A15" s="2" t="s">
         <v>131</v>
       </c>
@@ -1440,7 +1463,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" hidden="1">
+    <row r="16" spans="1:10" ht="28.5">
       <c r="A16" s="2" t="s">
         <v>130</v>
       </c>
@@ -1471,7 +1494,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="45" hidden="1">
+    <row r="17" spans="1:10" ht="28.5">
       <c r="A17" s="2" t="s">
         <v>113</v>
       </c>
@@ -1499,7 +1522,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="45" hidden="1">
+    <row r="18" spans="1:10" ht="28.5">
       <c r="A18" s="2" t="s">
         <v>114</v>
       </c>
@@ -1527,7 +1550,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30" hidden="1">
+    <row r="19" spans="1:10" ht="28.5">
       <c r="A19" s="4" t="s">
         <v>125</v>
       </c>
@@ -1555,7 +1578,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="45" hidden="1">
+    <row r="20" spans="1:10" ht="28.5">
       <c r="A20" s="4" t="s">
         <v>126</v>
       </c>
@@ -1583,7 +1606,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="45" hidden="1">
+    <row r="21" spans="1:10" ht="28.5">
       <c r="A21" s="4" t="s">
         <v>126</v>
       </c>
@@ -1611,7 +1634,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30" hidden="1">
+    <row r="22" spans="1:10" ht="28.5">
       <c r="A22" s="4" t="s">
         <v>127</v>
       </c>
@@ -1639,7 +1662,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" hidden="1">
+    <row r="23" spans="1:10" ht="28.5">
       <c r="A23" s="4" t="s">
         <v>128</v>
       </c>
@@ -1667,7 +1690,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" hidden="1">
+    <row r="24" spans="1:10" ht="28.5">
       <c r="A24" s="4" t="s">
         <v>127</v>
       </c>
@@ -1695,7 +1718,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="45" hidden="1">
+    <row r="25" spans="1:10" ht="42.75">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -1723,7 +1746,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="45" hidden="1">
+    <row r="26" spans="1:10" ht="42.75">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -1748,7 +1771,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="45" hidden="1">
+    <row r="27" spans="1:10" ht="28.5">
       <c r="A27" s="4" t="s">
         <v>123</v>
       </c>
@@ -1776,7 +1799,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="45" hidden="1">
+    <row r="28" spans="1:10" ht="28.5">
       <c r="A28" s="4" t="s">
         <v>124</v>
       </c>
@@ -1809,7 +1832,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="45" hidden="1">
+    <row r="29" spans="1:10" ht="28.5">
       <c r="A29" s="4" t="s">
         <v>124</v>
       </c>
@@ -1837,7 +1860,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="45" hidden="1">
+    <row r="30" spans="1:10" ht="28.5">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
@@ -1865,7 +1888,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="45" hidden="1">
+    <row r="31" spans="1:10" ht="42.75">
       <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
@@ -1893,7 +1916,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" hidden="1">
+    <row r="32" spans="1:10" ht="28.5">
       <c r="A32" s="4" t="s">
         <v>110</v>
       </c>
@@ -1921,7 +1944,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" hidden="1">
+    <row r="33" spans="1:10" ht="28.5">
       <c r="A33" s="4" t="s">
         <v>111</v>
       </c>
@@ -1949,7 +1972,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="45" hidden="1">
+    <row r="34" spans="1:10" ht="42.75">
       <c r="A34" s="4" t="s">
         <v>122</v>
       </c>
@@ -1974,7 +1997,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="45" hidden="1">
+    <row r="35" spans="1:10" ht="42.75">
       <c r="A35" s="4" t="s">
         <v>121</v>
       </c>
@@ -1999,7 +2022,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30" hidden="1">
+    <row r="36" spans="1:10" ht="28.5">
       <c r="A36" s="4" t="s">
         <v>112</v>
       </c>
@@ -2027,7 +2050,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="45">
+    <row r="37" spans="1:10" ht="42.75">
       <c r="A37" s="4" t="s">
         <v>120</v>
       </c>
@@ -2055,7 +2078,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="45">
+    <row r="38" spans="1:10" ht="42.75">
       <c r="A38" s="4" t="s">
         <v>119</v>
       </c>
@@ -2083,7 +2106,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="45">
+    <row r="39" spans="1:10" ht="42.75">
       <c r="A39" s="4" t="s">
         <v>118</v>
       </c>
@@ -2111,7 +2134,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="45">
+    <row r="40" spans="1:10" ht="28.5">
       <c r="A40" s="4" t="s">
         <v>117</v>
       </c>
@@ -2139,7 +2162,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="45">
+    <row r="41" spans="1:10" ht="28.5">
       <c r="A41" s="4" t="s">
         <v>115</v>
       </c>
@@ -2167,7 +2190,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="45">
+    <row r="42" spans="1:10" ht="28.5">
       <c r="A42" s="4" t="s">
         <v>116</v>
       </c>
@@ -2195,7 +2218,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="30" hidden="1">
+    <row r="43" spans="1:10" ht="28.5">
       <c r="A43" s="4" t="s">
         <v>133</v>
       </c>
@@ -2222,7 +2245,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="30" hidden="1">
+    <row r="44" spans="1:10" ht="28.5">
       <c r="A44" s="4" t="s">
         <v>134</v>
       </c>
@@ -2249,7 +2272,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="30" hidden="1">
+    <row r="45" spans="1:10" ht="28.5">
       <c r="A45" s="4" t="s">
         <v>135</v>
       </c>
@@ -2276,7 +2299,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1">
+    <row r="46" spans="1:10">
       <c r="A46" s="4" t="s">
         <v>67</v>
       </c>
@@ -2301,7 +2324,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="4" t="s">
         <v>68</v>
       </c>
@@ -2326,7 +2349,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="30" hidden="1">
+    <row r="48" spans="1:10" ht="28.5">
       <c r="A48" s="4" t="s">
         <v>69</v>
       </c>
@@ -2351,7 +2374,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="30" hidden="1">
+    <row r="49" spans="1:10" ht="28.5">
       <c r="A49" s="4" t="s">
         <v>70</v>
       </c>
@@ -2376,7 +2399,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="30" hidden="1">
+    <row r="50" spans="1:10" ht="28.5">
       <c r="A50" s="4" t="s">
         <v>77</v>
       </c>
@@ -2404,7 +2427,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="30" hidden="1">
+    <row r="51" spans="1:10">
       <c r="A51" s="4" t="s">
         <v>87</v>
       </c>
@@ -2432,7 +2455,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="30" hidden="1">
+    <row r="52" spans="1:10" ht="28.5">
       <c r="A52" s="4" t="s">
         <v>88</v>
       </c>
@@ -2460,7 +2483,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1">
+    <row r="53" spans="1:10">
       <c r="A53" s="4" t="s">
         <v>89</v>
       </c>
@@ -2488,7 +2511,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="30" hidden="1">
+    <row r="54" spans="1:10" ht="28.5">
       <c r="A54" s="4" t="s">
         <v>90</v>
       </c>
@@ -2516,7 +2539,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="30" hidden="1">
+    <row r="55" spans="1:10">
       <c r="A55" s="4" t="s">
         <v>91</v>
       </c>
@@ -2544,7 +2567,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="30" hidden="1">
+    <row r="56" spans="1:10" ht="28.5">
       <c r="A56" s="4" t="s">
         <v>92</v>
       </c>
@@ -2572,7 +2595,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="30" hidden="1">
+    <row r="57" spans="1:10" ht="28.5">
       <c r="A57" s="4" t="s">
         <v>93</v>
       </c>
@@ -2600,7 +2623,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="30" hidden="1">
+    <row r="58" spans="1:10" ht="28.5">
       <c r="A58" s="4" t="s">
         <v>94</v>
       </c>
@@ -2628,7 +2651,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="30" hidden="1">
+    <row r="59" spans="1:10" ht="28.5">
       <c r="A59" s="4" t="s">
         <v>95</v>
       </c>
@@ -2656,7 +2679,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="30" hidden="1">
+    <row r="60" spans="1:10" ht="28.5">
       <c r="A60" s="4" t="s">
         <v>96</v>
       </c>
@@ -2681,7 +2704,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="30" hidden="1">
+    <row r="61" spans="1:10" ht="28.5">
       <c r="A61" s="4" t="s">
         <v>98</v>
       </c>
@@ -2706,7 +2729,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="30" hidden="1">
+    <row r="62" spans="1:10" ht="28.5">
       <c r="A62" s="8" t="s">
         <v>100</v>
       </c>
@@ -2734,7 +2757,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="45" hidden="1">
+    <row r="63" spans="1:10" ht="28.5">
       <c r="A63" s="4" t="s">
         <v>101</v>
       </c>
@@ -2762,7 +2785,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="30" hidden="1">
+    <row r="64" spans="1:10" ht="28.5">
       <c r="A64" s="4" t="s">
         <v>104</v>
       </c>
@@ -2787,7 +2810,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="30" hidden="1">
+    <row r="65" spans="1:10" ht="28.5">
       <c r="A65" s="4" t="s">
         <v>105</v>
       </c>
@@ -2812,7 +2835,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="30" hidden="1">
+    <row r="66" spans="1:10" ht="28.5">
       <c r="A66" s="4" t="s">
         <v>106</v>
       </c>
@@ -2837,7 +2860,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="30" hidden="1">
+    <row r="67" spans="1:10" ht="28.5">
       <c r="A67" s="4" t="s">
         <v>136</v>
       </c>
@@ -2862,7 +2885,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="45" hidden="1">
+    <row r="68" spans="1:10" ht="42.75">
       <c r="A68" s="4" t="s">
         <v>137</v>
       </c>
@@ -2887,7 +2910,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="30" hidden="1">
+    <row r="69" spans="1:10" ht="28.5">
       <c r="A69" s="4" t="s">
         <v>141</v>
       </c>
@@ -2912,13 +2935,115 @@
         <v>146</v>
       </c>
     </row>
+    <row r="70" spans="1:10" ht="28.5">
+      <c r="A70" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" s="4">
+        <v>6</v>
+      </c>
+      <c r="E70" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H70" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I70" s="4">
+        <v>3</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="28.5">
+      <c r="A71" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D71" s="4">
+        <v>6</v>
+      </c>
+      <c r="E71" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H71" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I71" s="4">
+        <v>3</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="28.5">
+      <c r="A72" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D72" s="4">
+        <v>6</v>
+      </c>
+      <c r="E72" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H72" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="28.5">
+      <c r="A73" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D73" s="4">
+        <v>6</v>
+      </c>
+      <c r="E73" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H73" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J69">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="PRAC"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="9"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Merged process identifiers into doctype code list; TICC-95
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$J$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$K$73</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="190">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -381,9 +381,6 @@
     <t>Procurement procedure subscription Request V1</t>
   </si>
   <si>
-    <t>DHSC Customized  Ordering profile OrderResponse V1</t>
-  </si>
-  <si>
     <t>DHSC Customized Ordering profile Order V1</t>
   </si>
   <si>
@@ -486,13 +483,121 @@
     <t>Profile name</t>
   </si>
   <si>
-    <t>PEPPOL Document Type Identifier Scheme</t>
-  </si>
-  <si>
-    <t>PEPPOL Document Type Identifier Value</t>
-  </si>
-  <si>
     <t>Issued by OpenPEPPOL?</t>
+  </si>
+  <si>
+    <t>DHSC Customized Ordering profile OrderResponse V1</t>
+  </si>
+  <si>
+    <t>Peppol Document Type Identifier Scheme</t>
+  </si>
+  <si>
+    <t>Peppol Document Type Identifier Value</t>
+  </si>
+  <si>
+    <t>Associated Process Identifier(s)</t>
+  </si>
+  <si>
+    <t>oioubl-procid-ubl::Reference-Utility-1.0</t>
+  </si>
+  <si>
+    <t>oioubl-procid-ubl::Procurement-ReminderOnly-1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:poacc:billing:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.peppol.eu:profile:bis63a:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:catalogue_only:3
+cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:catalogue_wo_response:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:catalogue_only:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:ordering:3
+cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:order_only:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:invoice_response:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:punch_out:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:ordering:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:despatch_advice:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:order_agreement:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:mlr:3</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:www.efaktura.gov.pl:ver1.0:account_corr:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:www.efaktura.gov.pl:ver1.0:corr_inv:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:www.efaktura.gov.pl:ver1.0:receipt_advice:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:pracc:p003:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:pracc:p002:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:pracc:p001:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::none</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii01:ver1.0
+cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii01:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii01:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii01:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii03:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii03:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii04:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii04:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii05:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii05:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii06:ver1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii28:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii30:ver2.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii36:ver2.0</t>
   </si>
 </sst>
 </file>
@@ -558,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -581,8 +686,11 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -983,35 +1091,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.36328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="47.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="4" customWidth="1"/>
-    <col min="3" max="3" width="103.1328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="47.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="103.08984375" style="4" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.73046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.86328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.3984375" style="4"/>
+    <col min="5" max="5" width="14.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.36328125" style="4"/>
+    <col min="11" max="11" width="64.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.36328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="42.75">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="29">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
@@ -1023,19 +1132,22 @@
         <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="42.75">
+      <c r="K1" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="43.5">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1063,10 +1175,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="42.75">
+        <v>141</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1094,10 +1209,13 @@
         <v>1</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="43.5">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1125,12 +1243,15 @@
         <v>1</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="29">
       <c r="A5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>60</v>
@@ -1158,10 +1279,13 @@
       <c r="J5" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="28.5">
+      <c r="K5" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="43.5">
       <c r="A6" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>60</v>
@@ -1189,10 +1313,13 @@
       <c r="J6" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="28.5">
+      <c r="K6" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="43.5">
       <c r="A7" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>60</v>
@@ -1220,8 +1347,11 @@
       <c r="J7" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="28.5">
+      <c r="K7" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="29">
       <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
@@ -1248,8 +1378,11 @@
       <c r="J8" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="28.5">
+      <c r="K8" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="29">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1277,10 +1410,13 @@
         <v>1</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="29">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1311,10 +1447,13 @@
         <v>2</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="29">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1339,10 +1478,13 @@
         <v>2</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="29">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1370,10 +1512,13 @@
         <v>1</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="29">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1398,12 +1543,15 @@
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="29">
       <c r="A14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>60</v>
@@ -1429,12 +1577,15 @@
         <v>1</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29">
       <c r="A15" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>60</v>
@@ -1460,12 +1611,15 @@
         <v>1</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29">
       <c r="A16" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>60</v>
@@ -1491,10 +1645,13 @@
         <v>1</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="29">
       <c r="A17" s="2" t="s">
         <v>110</v>
       </c>
@@ -1519,10 +1676,13 @@
         <v>2</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="29">
       <c r="A18" s="2" t="s">
         <v>111</v>
       </c>
@@ -1547,12 +1707,15 @@
         <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="29">
       <c r="A19" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>60</v>
@@ -1575,12 +1738,15 @@
         <v>1</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="43.5">
       <c r="A20" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>60</v>
@@ -1603,12 +1769,15 @@
         <v>1</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="43.5">
       <c r="A21" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>60</v>
@@ -1631,12 +1800,15 @@
         <v>1</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="29">
       <c r="A22" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>60</v>
@@ -1659,12 +1831,15 @@
         <v>1</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="29">
       <c r="A23" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>60</v>
@@ -1687,12 +1862,15 @@
         <v>1</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="29">
       <c r="A24" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>60</v>
@@ -1715,10 +1893,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="43.5">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -1743,10 +1924,13 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="43.5">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -1768,12 +1952,15 @@
         <v>0</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="29">
       <c r="A27" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>60</v>
@@ -1796,12 +1983,15 @@
         <v>1</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="29">
       <c r="A28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>60</v>
@@ -1829,12 +2019,15 @@
         <v>1</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="43.5">
       <c r="A29" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>60</v>
@@ -1857,10 +2050,13 @@
         <v>1</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="43.5">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
@@ -1885,10 +2081,13 @@
         <v>1</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="43.5">
       <c r="A31" s="4" t="s">
         <v>41</v>
       </c>
@@ -1913,10 +2112,13 @@
         <v>1</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="29">
       <c r="A32" s="4" t="s">
         <v>107</v>
       </c>
@@ -1941,10 +2143,13 @@
         <v>3</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="29">
       <c r="A33" s="4" t="s">
         <v>108</v>
       </c>
@@ -1969,12 +2174,15 @@
         <v>3</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="43.5">
       <c r="A34" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>60</v>
@@ -1994,12 +2202,15 @@
         <v>0</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="43.5">
       <c r="A35" s="4" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>60</v>
@@ -2019,10 +2230,13 @@
         <v>0</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="29">
       <c r="A36" s="4" t="s">
         <v>109</v>
       </c>
@@ -2047,10 +2261,13 @@
         <v>3</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="43.5">
       <c r="A37" s="4" t="s">
         <v>117</v>
       </c>
@@ -2075,10 +2292,13 @@
         <v>1</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="42.75">
+        <v>141</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="43.5">
       <c r="A38" s="4" t="s">
         <v>116</v>
       </c>
@@ -2103,10 +2323,13 @@
         <v>1</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="42.75">
+        <v>141</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="43.5">
       <c r="A39" s="4" t="s">
         <v>115</v>
       </c>
@@ -2131,10 +2354,13 @@
         <v>1</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="43.5">
       <c r="A40" s="4" t="s">
         <v>114</v>
       </c>
@@ -2159,10 +2385,13 @@
         <v>1</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="43.5">
       <c r="A41" s="4" t="s">
         <v>112</v>
       </c>
@@ -2187,10 +2416,13 @@
         <v>1</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="29">
       <c r="A42" s="4" t="s">
         <v>113</v>
       </c>
@@ -2215,12 +2447,15 @@
         <v>1</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="28.5">
+        <v>141</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="29">
       <c r="A43" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>60</v>
@@ -2242,12 +2477,15 @@
         <v>0</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="29">
       <c r="A44" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>60</v>
@@ -2269,12 +2507,15 @@
         <v>0</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="29">
       <c r="A45" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>60</v>
@@ -2296,10 +2537,13 @@
         <v>0</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="4" t="s">
         <v>65</v>
       </c>
@@ -2321,10 +2565,13 @@
         <v>0</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="4" t="s">
         <v>66</v>
       </c>
@@ -2346,10 +2593,13 @@
         <v>0</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="29">
       <c r="A48" s="4" t="s">
         <v>67</v>
       </c>
@@ -2371,10 +2621,13 @@
         <v>0</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="29">
       <c r="A49" s="4" t="s">
         <v>68</v>
       </c>
@@ -2396,10 +2649,13 @@
         <v>0</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="29">
       <c r="A50" s="4" t="s">
         <v>74</v>
       </c>
@@ -2424,10 +2680,13 @@
         <v>1</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="29">
       <c r="A51" s="4" t="s">
         <v>84</v>
       </c>
@@ -2452,10 +2711,13 @@
         <v>3</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="29">
       <c r="A52" s="4" t="s">
         <v>85</v>
       </c>
@@ -2480,10 +2742,13 @@
         <v>3</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="29">
       <c r="A53" s="4" t="s">
         <v>86</v>
       </c>
@@ -2508,10 +2773,13 @@
         <v>3</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="29">
       <c r="A54" s="4" t="s">
         <v>87</v>
       </c>
@@ -2536,10 +2804,13 @@
         <v>3</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>142</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="4" t="s">
         <v>88</v>
       </c>
@@ -2564,10 +2835,13 @@
         <v>3</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="29">
       <c r="A56" s="4" t="s">
         <v>89</v>
       </c>
@@ -2592,10 +2866,13 @@
         <v>3</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="29">
       <c r="A57" s="4" t="s">
         <v>90</v>
       </c>
@@ -2620,10 +2897,13 @@
         <v>3</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K57" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="29">
       <c r="A58" s="4" t="s">
         <v>91</v>
       </c>
@@ -2648,10 +2928,13 @@
         <v>3</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="29">
       <c r="A59" s="4" t="s">
         <v>92</v>
       </c>
@@ -2676,10 +2959,13 @@
         <v>3</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="29">
       <c r="A60" s="4" t="s">
         <v>93</v>
       </c>
@@ -2701,10 +2987,13 @@
         <v>0</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="29">
       <c r="A61" s="4" t="s">
         <v>95</v>
       </c>
@@ -2726,11 +3015,14 @@
         <v>0</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="28.5">
-      <c r="A62" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="29">
+      <c r="A62" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -2754,10 +3046,13 @@
         <v>3</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="29">
       <c r="A63" s="4" t="s">
         <v>98</v>
       </c>
@@ -2782,10 +3077,13 @@
         <v>3</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K63" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="29">
       <c r="A64" s="4" t="s">
         <v>101</v>
       </c>
@@ -2807,10 +3105,13 @@
         <v>0</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K64" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="29">
       <c r="A65" s="4" t="s">
         <v>102</v>
       </c>
@@ -2832,10 +3133,13 @@
         <v>0</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K65" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="29">
       <c r="A66" s="4" t="s">
         <v>103</v>
       </c>
@@ -2857,18 +3161,21 @@
         <v>0</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K66" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="29">
       <c r="A67" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67" s="4">
         <v>6</v>
@@ -2882,18 +3189,21 @@
         <v>0</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="42.75">
+        <v>142</v>
+      </c>
+      <c r="K67" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="43.5">
       <c r="A68" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="D68" s="4">
         <v>6</v>
@@ -2907,18 +3217,21 @@
         <v>0</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K68" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="29">
       <c r="A69" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D69" s="4">
         <v>6</v>
@@ -2932,18 +3245,21 @@
         <v>0</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="28.5">
-      <c r="A70" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
+      </c>
+      <c r="K69" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="29">
+      <c r="A70" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D70" s="4">
         <v>6</v>
@@ -2960,18 +3276,21 @@
         <v>3</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="28.5">
-      <c r="A71" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="K70" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="29">
+      <c r="A71" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D71" s="4">
         <v>6</v>
@@ -2988,18 +3307,21 @@
         <v>3</v>
       </c>
       <c r="J71" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K71" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="29">
+      <c r="A72" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="28.5">
-      <c r="A72" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="B72" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D72" s="4">
         <v>6</v>
@@ -3013,18 +3335,21 @@
         <v>0</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="28.5">
+        <v>142</v>
+      </c>
+      <c r="K72" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="43.5">
       <c r="A73" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D73" s="4">
         <v>6</v>
@@ -3038,13 +3363,14 @@
         <v>0</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="K73" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J69">
-    <filterColumn colId="9"/>
-  </autoFilter>
+  <autoFilter ref="A1:K73"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added SI 1.2 - TICC-107
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="196">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -493,9 +493,6 @@
   </si>
   <si>
     <t>Peppol Document Type Identifier Value</t>
-  </si>
-  <si>
-    <t>Associated Process Identifier(s)</t>
   </si>
   <si>
     <t>oioubl-procid-ubl::Reference-Utility-1.0</t>
@@ -598,6 +595,28 @@
   </si>
   <si>
     <t>cenbii-procid-ubl::urn:www.cenbii.eu:profile:bii36:ver2.0</t>
+  </si>
+  <si>
+    <t>Associated Process/Profile Identifier(s)
+(Format scheme::value)</t>
+  </si>
+  <si>
+    <t>SI-UBL 1.2 Invoice</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:www.cenbii.eu:transaction:biitrns010:ver2.0:extended:urn:www.peppol.eu:bis:peppol4a:ver2.0:extended:urn:www.simplerinvoicing.org:si:si-ubl:ver1.2::2.1</t>
+  </si>
+  <si>
+    <t>urn:www.cenbii.eu:profile:bii04:ver1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:www.cenbii.eu:transaction:biitrns001:ver2.0:extended:urn:www.peppol.eu:bis:peppol3a:ver2.0:extended:urn:www.simplerinvoicing.org:si:si-ubl:ver1.2::2.1</t>
+  </si>
+  <si>
+    <t>SI-UBL 1.2 Order</t>
+  </si>
+  <si>
+    <t>urn:www.cenbii.eu:profile:bii03:ver2.0</t>
   </si>
 </sst>
 </file>
@@ -1091,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="D64" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.36328125" defaultRowHeight="14.5"/>
@@ -1144,7 +1163,7 @@
         <v>140</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="43.5">
@@ -1178,7 +1197,7 @@
         <v>141</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.5">
@@ -1212,7 +1231,7 @@
         <v>141</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.5">
@@ -1246,7 +1265,7 @@
         <v>141</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="29">
@@ -1280,7 +1299,7 @@
         <v>142</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.5">
@@ -1314,7 +1333,7 @@
         <v>142</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="43.5">
@@ -1348,7 +1367,7 @@
         <v>142</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="29">
@@ -1379,7 +1398,7 @@
         <v>142</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="29">
@@ -1413,7 +1432,7 @@
         <v>142</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="29">
@@ -1450,7 +1469,7 @@
         <v>142</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="29">
@@ -1481,7 +1500,7 @@
         <v>142</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="29">
@@ -1515,7 +1534,7 @@
         <v>142</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="29">
@@ -1546,7 +1565,7 @@
         <v>142</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="29">
@@ -1580,7 +1599,7 @@
         <v>142</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="29">
@@ -1614,7 +1633,7 @@
         <v>142</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="29">
@@ -1648,7 +1667,7 @@
         <v>142</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="29">
@@ -1679,7 +1698,7 @@
         <v>142</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="29">
@@ -1710,7 +1729,7 @@
         <v>142</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="29">
@@ -1741,7 +1760,7 @@
         <v>142</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="43.5">
@@ -1772,7 +1791,7 @@
         <v>142</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="43.5">
@@ -1803,7 +1822,7 @@
         <v>142</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="29">
@@ -1834,7 +1853,7 @@
         <v>142</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="29">
@@ -1865,7 +1884,7 @@
         <v>142</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="29">
@@ -1896,7 +1915,7 @@
         <v>142</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="43.5">
@@ -1927,7 +1946,7 @@
         <v>142</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="43.5">
@@ -1955,7 +1974,7 @@
         <v>142</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="29">
@@ -1986,7 +2005,7 @@
         <v>142</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="29">
@@ -2022,7 +2041,7 @@
         <v>142</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="43.5">
@@ -2053,7 +2072,7 @@
         <v>142</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="43.5">
@@ -2084,7 +2103,7 @@
         <v>142</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="43.5">
@@ -2115,7 +2134,7 @@
         <v>142</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="29">
@@ -2146,7 +2165,7 @@
         <v>142</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="29">
@@ -2177,7 +2196,7 @@
         <v>142</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="43.5">
@@ -2205,7 +2224,7 @@
         <v>142</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="43.5">
@@ -2233,7 +2252,7 @@
         <v>142</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="29">
@@ -2264,7 +2283,7 @@
         <v>142</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="43.5">
@@ -2295,7 +2314,7 @@
         <v>141</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="43.5">
@@ -2326,7 +2345,7 @@
         <v>141</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="43.5">
@@ -2357,7 +2376,7 @@
         <v>141</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="43.5">
@@ -2388,7 +2407,7 @@
         <v>141</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="43.5">
@@ -2419,7 +2438,7 @@
         <v>141</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="29">
@@ -2450,7 +2469,7 @@
         <v>141</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="29">
@@ -2480,7 +2499,7 @@
         <v>142</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="29">
@@ -2510,7 +2529,7 @@
         <v>142</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="29">
@@ -2540,7 +2559,7 @@
         <v>142</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2568,7 +2587,7 @@
         <v>142</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2596,7 +2615,7 @@
         <v>142</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="29">
@@ -2624,7 +2643,7 @@
         <v>142</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="29">
@@ -2652,7 +2671,7 @@
         <v>142</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="29">
@@ -2683,7 +2702,7 @@
         <v>142</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="29">
@@ -2714,7 +2733,7 @@
         <v>142</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="29">
@@ -2745,7 +2764,7 @@
         <v>142</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="29">
@@ -2776,7 +2795,7 @@
         <v>142</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="29">
@@ -2807,7 +2826,7 @@
         <v>142</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2838,7 +2857,7 @@
         <v>142</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29">
@@ -2869,7 +2888,7 @@
         <v>142</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="29">
@@ -2900,7 +2919,7 @@
         <v>142</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="29">
@@ -2931,7 +2950,7 @@
         <v>142</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="29">
@@ -2962,7 +2981,7 @@
         <v>142</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="29">
@@ -2990,7 +3009,7 @@
         <v>142</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="29">
@@ -3018,7 +3037,7 @@
         <v>142</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="29">
@@ -3049,7 +3068,7 @@
         <v>142</v>
       </c>
       <c r="K62" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="29">
@@ -3080,7 +3099,7 @@
         <v>142</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="29">
@@ -3108,7 +3127,7 @@
         <v>142</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="29">
@@ -3136,7 +3155,7 @@
         <v>142</v>
       </c>
       <c r="K65" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="29">
@@ -3164,7 +3183,7 @@
         <v>142</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="29">
@@ -3192,7 +3211,7 @@
         <v>142</v>
       </c>
       <c r="K67" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="43.5">
@@ -3220,7 +3239,7 @@
         <v>142</v>
       </c>
       <c r="K68" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="29">
@@ -3248,7 +3267,7 @@
         <v>142</v>
       </c>
       <c r="K69" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="29">
@@ -3279,7 +3298,7 @@
         <v>142</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="29">
@@ -3310,7 +3329,7 @@
         <v>142</v>
       </c>
       <c r="K71" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="29">
@@ -3338,7 +3357,7 @@
         <v>142</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="43.5">
@@ -3366,7 +3385,63 @@
         <v>142</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="43.5">
+      <c r="A74" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D74" s="4">
+        <v>6</v>
+      </c>
+      <c r="E74" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H74" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="43.5">
+      <c r="A75" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D75" s="4">
+        <v>6</v>
+      </c>
+      <c r="E75" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H75" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed "SG PEPPOL BIS Billing 3.0 Credit Note" ID
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v6 draft.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$K$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$K$74</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="197">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>urn:www.cenbii.eu:profile:bii03:ver2.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:fdc:peppol.eu:2017:poacc:billing:international:sg:3.0::2.1</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D64" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.36328125" defaultRowHeight="14.5"/>
@@ -3085,8 +3088,14 @@
         <v>4</v>
       </c>
       <c r="E63" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F63" s="4">
+        <v>6</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="H63" s="4" t="b">
         <f>TRUE</f>
@@ -3104,24 +3113,27 @@
     </row>
     <row r="64" spans="1:11" ht="29">
       <c r="A64" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>104</v>
+        <v>196</v>
       </c>
       <c r="D64" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E64" s="4" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="H64" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I64" s="4">
+        <v>3</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>142</v>
@@ -3132,13 +3144,13 @@
     </row>
     <row r="65" spans="1:11" ht="29">
       <c r="A65" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D65" s="4">
         <v>5</v>
@@ -3160,13 +3172,13 @@
     </row>
     <row r="66" spans="1:11" ht="29">
       <c r="A66" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D66" s="4">
         <v>5</v>
@@ -3188,41 +3200,41 @@
     </row>
     <row r="67" spans="1:11" ht="29">
       <c r="A67" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" s="4">
+        <v>5</v>
+      </c>
+      <c r="E67" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K67" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="29">
+      <c r="A68" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C67" s="4" t="s">
+      <c r="B68" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="D67" s="4">
-        <v>6</v>
-      </c>
-      <c r="E67" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H67" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K67" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="43.5">
-      <c r="A68" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="D68" s="4">
         <v>6</v>
@@ -3239,18 +3251,18 @@
         <v>142</v>
       </c>
       <c r="K68" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="29">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="43.5">
       <c r="A69" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D69" s="4">
         <v>6</v>
@@ -3267,18 +3279,18 @@
         <v>142</v>
       </c>
       <c r="K69" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="29">
-      <c r="A70" s="9" t="s">
-        <v>145</v>
+      <c r="A70" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D70" s="4">
         <v>6</v>
@@ -3288,28 +3300,25 @@
         <v>0</v>
       </c>
       <c r="H70" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I70" s="4">
-        <v>3</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>142</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="29">
       <c r="A71" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D71" s="4">
         <v>6</v>
@@ -3333,14 +3342,14 @@
       </c>
     </row>
     <row r="72" spans="1:11" ht="29">
-      <c r="A72" s="4" t="s">
-        <v>143</v>
+      <c r="A72" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D72" s="4">
         <v>6</v>
@@ -3350,8 +3359,11 @@
         <v>0</v>
       </c>
       <c r="H72" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I72" s="4">
+        <v>3</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>142</v>
@@ -3360,15 +3372,15 @@
         <v>158</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="43.5">
+    <row r="73" spans="1:11" ht="29">
       <c r="A73" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D73" s="4">
         <v>6</v>
@@ -3390,13 +3402,13 @@
     </row>
     <row r="74" spans="1:11" ht="43.5">
       <c r="A74" s="4" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="D74" s="4">
         <v>6</v>
@@ -3412,19 +3424,19 @@
       <c r="J74" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="K74" s="4" t="s">
-        <v>192</v>
+      <c r="K74" s="8" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="43.5">
       <c r="A75" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D75" s="4">
         <v>6</v>
@@ -3441,11 +3453,39 @@
         <v>142</v>
       </c>
       <c r="K75" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="43.5">
+      <c r="A76" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D76" s="4">
+        <v>6</v>
+      </c>
+      <c r="E76" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H76" s="4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K76" s="4" t="s">
         <v>195</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K73"/>
+  <autoFilter ref="A1:K74"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>